<commit_message>
Updated documentation for expert review
</commit_message>
<xml_diff>
--- a/Documentation/Semaine 3/Journal de travail Renaud Grégory TPI.xlsx
+++ b/Documentation/Semaine 3/Journal de travail Renaud Grégory TPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/ph62ldr_eduvaud_ch/Documents/TPI/Semaine 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{E93AF827-F335-4273-9BF2-1B7E35411D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B3F4D1D-777D-4757-93EB-6C7F0E275A96}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{E93AF827-F335-4273-9BF2-1B7E35411D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94CAC427-59AE-40C5-A1C1-9E3E6D7102E5}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{E616EBF9-A1E1-4B05-B307-B39FC77B0801}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="200">
   <si>
     <t>Date</t>
   </si>
@@ -548,6 +548,99 @@
   </si>
   <si>
     <t>Préparation des documents pour le 5ème rendu</t>
+  </si>
+  <si>
+    <t>Modification de l'affichage des labels pour les charts</t>
+  </si>
+  <si>
+    <t>Prend les valeurs en français au lieux des champs direct de la DB</t>
+  </si>
+  <si>
+    <t>Entretien avec Monsieur Rochat pour retour sur l'application</t>
+  </si>
+  <si>
+    <t>Commentaire du code</t>
+  </si>
+  <si>
+    <t>Commentaire pour le format doxygen</t>
+  </si>
+  <si>
+    <t>Relecture et correction du rapport</t>
+  </si>
+  <si>
+    <t>Bloqué car impossible de push l'application sur Azure (problème de connexion)</t>
+  </si>
+  <si>
+    <t>Problème de 2FA</t>
+  </si>
+  <si>
+    <t>Entretien avec Monsieur Wulliamoz concernant le problème de 2FA</t>
+  </si>
+  <si>
+    <t>Réglé</t>
+  </si>
+  <si>
+    <t>Adaptation de certain affichage pour le mobile.</t>
+  </si>
+  <si>
+    <t>Formulaire de nouvel entrée en horizontal au lieux de vertical.</t>
+  </si>
+  <si>
+    <t>Entretien avec le chef de projet pour des questions</t>
+  </si>
+  <si>
+    <t>Question concernant la vérification d'entrées sur les différentes années.</t>
+  </si>
+  <si>
+    <t>Modification de l'affichage des stats en fonction de l'année.</t>
+  </si>
+  <si>
+    <t>Je dois changer toute ma logique de réception des données de la DB.</t>
+  </si>
+  <si>
+    <t>Entretien téléphonique concernant l'hébergement</t>
+  </si>
+  <si>
+    <t>Ajout de nouveaux test d'entrée erronées. Il ne me manque plus que la gestion de l'année courante à l'affichage.</t>
+  </si>
+  <si>
+    <t>Test par Mme Andolfato</t>
+  </si>
+  <si>
+    <t>Modification de la validation des champs pour les entrées de temps pour les séances</t>
+  </si>
+  <si>
+    <t>Modification de l'affichage des donnée uniquement de l'année scolaire courante.</t>
+  </si>
+  <si>
+    <t>La partie statistique va me prendre pas mal plus de temps car mes classes DAO ne sont pas encore faites pour récupérer des données d'une année scolaire spécifique.</t>
+  </si>
+  <si>
+    <t>Ajout d'un dropdown dynamique en fonction des entrées de la BD.</t>
+  </si>
+  <si>
+    <t>Modification de l'affichage des charts pour un affichage dynamique en fonction de l'années sélectionnée.</t>
+  </si>
+  <si>
+    <t>Ne marche pas encore, je dois encore vérifier des valeurs de retours de la DB.</t>
+  </si>
+  <si>
+    <t>Finalisation de l'affichage dynamique des années pour les charts.</t>
+  </si>
+  <si>
+    <t>Certaines valeurs de retours étaient mal gérées et faisaient des erreurs de vérification après.</t>
+  </si>
+  <si>
+    <t>Sprint review finale</t>
+  </si>
+  <si>
+    <t>Les développement est fini, il ne me reste plus que la documentation. L'aplication à été testée par Monsieur Benzonana pour vérifier des cas d'erreurs.</t>
+  </si>
+  <si>
+    <t>Rédaction deu début de la phase de test</t>
+  </si>
+  <si>
+    <t>Préparation de la documentation pour l'envoi aux experts N°6</t>
   </si>
 </sst>
 </file>
@@ -556,8 +649,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd:hh:mm"/>
-    <numFmt numFmtId="167" formatCode="dd&quot;J&quot;\ hh&quot;H&quot;\ &quot;&quot;mm&quot;M&quot;"/>
-    <numFmt numFmtId="168" formatCode="[h]:mm"/>
+    <numFmt numFmtId="165" formatCode="dd&quot;J&quot;\ hh&quot;H&quot;\ &quot;&quot;mm&quot;M&quot;"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -682,8 +775,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1213,19 +1306,19 @@
                 <c:formatCode>dd:hh:mm</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.28125</c:v>
+                  <c:v>1.6701388888888897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42013888888888878</c:v>
+                  <c:v>0.47569444444444436</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.10069444444444448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1388888888888889</c:v>
+                  <c:v>0.15972222222222221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25347222222222227</c:v>
+                  <c:v>0.31944444444444442</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.36458333333333326</c:v>
@@ -2237,8 +2330,8 @@
   <dimension ref="A1:I1196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4024,7 +4117,9 @@
         <f t="shared" si="4"/>
         <v>1.3888888888888895E-2</v>
       </c>
-      <c r="E70" s="5"/>
+      <c r="E70" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="F70" s="9" t="s">
         <v>129</v>
       </c>
@@ -4710,296 +4805,522 @@
       <c r="H97" s="9"/>
       <c r="I97" s="14"/>
     </row>
-    <row r="98" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
+    <row r="98" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B98" s="4">
+        <v>0.34375</v>
+      </c>
+      <c r="C98" s="4">
+        <v>0.375</v>
+      </c>
       <c r="D98" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E98" s="5"/>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="H98" s="9"/>
       <c r="I98" s="14"/>
     </row>
-    <row r="99" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="5"/>
+    <row r="99" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B99" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="C99" s="4">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="D99" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E99" s="5"/>
-      <c r="F99" s="9"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>171</v>
+      </c>
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
       <c r="I99" s="14"/>
     </row>
     <row r="100" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
+      <c r="A100" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B100" s="4">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C100" s="4">
+        <v>0.40972222222222221</v>
+      </c>
       <c r="D100" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E100" s="5"/>
-      <c r="F100" s="9"/>
-      <c r="G100" s="9"/>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="H100" s="9"/>
       <c r="I100" s="14"/>
     </row>
     <row r="101" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
+      <c r="A101" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B101" s="4">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0.44791666666666669</v>
+      </c>
       <c r="D101" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E101" s="5"/>
-      <c r="F101" s="9"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="G101" s="9"/>
       <c r="H101" s="9"/>
       <c r="I101" s="14"/>
     </row>
     <row r="102" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="5"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
+      <c r="A102" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B102" s="4">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C102" s="4">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="D102" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E102" s="5"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G102" s="10"/>
       <c r="H102" s="9"/>
       <c r="I102" s="14"/>
     </row>
-    <row r="103" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="5"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
+    <row r="103" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B103" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C103" s="4">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D103" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="E103" s="5"/>
-      <c r="F103" s="9"/>
-      <c r="G103" s="9"/>
+      <c r="F103" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="H103" s="9"/>
       <c r="I103" s="14"/>
     </row>
-    <row r="104" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
+    <row r="104" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B104" s="4">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C104" s="4">
+        <v>0.5625</v>
+      </c>
       <c r="D104" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="E104" s="5"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
+      <c r="F104" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>178</v>
+      </c>
       <c r="H104" s="9"/>
       <c r="I104" s="14"/>
     </row>
-    <row r="105" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
+    <row r="105" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B105" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C105" s="4">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="D105" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E105" s="5"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G105" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="H105" s="9"/>
       <c r="I105" s="14"/>
     </row>
-    <row r="106" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
+    <row r="106" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B106" s="4">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C106" s="4">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D106" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E106" s="5"/>
-      <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>182</v>
+      </c>
       <c r="H106" s="9"/>
       <c r="I106" s="14"/>
     </row>
-    <row r="107" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="5"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
+    <row r="107" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <v>45784</v>
+      </c>
+      <c r="B107" s="4">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="C107" s="4">
+        <v>0.65972222222222221</v>
+      </c>
       <c r="D107" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E107" s="5"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>184</v>
+      </c>
       <c r="H107" s="9"/>
       <c r="I107" s="14"/>
     </row>
     <row r="108" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="5"/>
+      <c r="A108" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B108" s="4">
+        <v>0.34375</v>
+      </c>
+      <c r="C108" s="4">
+        <v>0.35069444444444442</v>
+      </c>
       <c r="D108" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="E108" s="5"/>
-      <c r="F108" s="9"/>
+      <c r="F108" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G108" s="9"/>
       <c r="H108" s="9"/>
       <c r="I108" s="14"/>
     </row>
-    <row r="109" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="5"/>
+    <row r="109" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B109" s="4">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0.40277777777777779</v>
+      </c>
       <c r="D109" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E109" s="5"/>
-      <c r="F109" s="9"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="G109" s="9"/>
       <c r="H109" s="9"/>
       <c r="I109" s="14"/>
     </row>
     <row r="110" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
+      <c r="A110" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B110" s="4">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="C110" s="4">
+        <v>0.41319444444444442</v>
+      </c>
       <c r="D110" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E110" s="5"/>
-      <c r="F110" s="9"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="G110" s="9"/>
       <c r="H110" s="9"/>
       <c r="I110" s="14"/>
     </row>
-    <row r="111" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="5"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
+    <row r="111" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B111" s="4">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="C111" s="4">
+        <v>0.43055555555555558</v>
+      </c>
       <c r="D111" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E111" s="5"/>
-      <c r="F111" s="9"/>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="G111" s="9"/>
       <c r="H111" s="9"/>
       <c r="I111" s="14"/>
     </row>
-    <row r="112" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
+    <row r="112" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B112" s="4">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C112" s="4">
+        <v>0.44097222222222221</v>
+      </c>
       <c r="D112" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E112" s="5"/>
-      <c r="F112" s="9"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>189</v>
+      </c>
       <c r="G112" s="9"/>
-      <c r="H112" s="9"/>
+      <c r="H112" s="9" t="s">
+        <v>190</v>
+      </c>
       <c r="I112" s="14"/>
     </row>
-    <row r="113" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
+    <row r="113" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B113" s="4">
+        <v>0.44097222222222221</v>
+      </c>
+      <c r="C113" s="4">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="D113" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E113" s="5"/>
-      <c r="F113" s="9"/>
+        <v>3.8194444444444475E-2</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>191</v>
+      </c>
       <c r="G113" s="9"/>
       <c r="H113" s="9"/>
       <c r="I113" s="14"/>
     </row>
-    <row r="114" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
+    <row r="114" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>45785</v>
+      </c>
+      <c r="B114" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C114" s="4">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D114" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E114" s="5"/>
-      <c r="F114" s="9"/>
-      <c r="G114" s="9"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G114" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="H114" s="9"/>
       <c r="I114" s="14"/>
     </row>
-    <row r="115" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
+    <row r="115" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <v>45786</v>
+      </c>
+      <c r="B115" s="4">
+        <v>0.34375</v>
+      </c>
+      <c r="C115" s="4">
+        <v>0.40277777777777779</v>
+      </c>
       <c r="D115" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E115" s="5"/>
-      <c r="F115" s="9"/>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>194</v>
+      </c>
       <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
+      <c r="H115" s="9" t="s">
+        <v>195</v>
+      </c>
       <c r="I115" s="14"/>
     </row>
-    <row r="116" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
+    <row r="116" spans="1:9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>45786</v>
+      </c>
+      <c r="B116" s="4">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="C116" s="4">
+        <v>0.4548611111111111</v>
+      </c>
       <c r="D116" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E116" s="5"/>
-      <c r="F116" s="9"/>
-      <c r="G116" s="9"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G116" s="9" t="s">
+        <v>197</v>
+      </c>
       <c r="H116" s="9"/>
       <c r="I116" s="14"/>
     </row>
     <row r="117" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
+      <c r="A117" s="3">
+        <v>45786</v>
+      </c>
+      <c r="B117" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C117" s="4">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="D117" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E117" s="5"/>
-      <c r="F117" s="9"/>
+        <v>1.7361111111111105E-2</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>198</v>
+      </c>
       <c r="G117" s="9"/>
       <c r="H117" s="9"/>
       <c r="I117" s="14"/>
     </row>
-    <row r="118" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
+    <row r="118" spans="1:9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
+        <v>45786</v>
+      </c>
+      <c r="B118" s="4">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="C118" s="4">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="D118" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E118" s="5"/>
-      <c r="F118" s="9"/>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="G118" s="9"/>
       <c r="H118" s="9"/>
       <c r="I118" s="14"/>
@@ -17689,7 +18010,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H2 H2:I20 E3:H3 A3:D9 E4 E7:H9 H21 H22:I69 A34:E34 G34:H34 A35:H47 A48:B48 D48:H48 A49:H49 A50:E50 G50:H50 A51:H978 H71:I977">
+  <conditionalFormatting sqref="A2:H2 H2:I20 E3:H3 A3:D9 E4 E7:H9 H21 H22:I69 A34:E34 G34:H34 A35:H47 A48:B48 D48:H48 A49:H49 A50:E50 G50:H50 A51:H101 H71:I977 A102:F102 A103:H978">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
@@ -17730,7 +18051,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17754,7 +18075,7 @@
       </c>
       <c r="E1" s="17">
         <f>SUM(B2:B7)</f>
-        <v>2.5590277777777777</v>
+        <v>3.0902777777777786</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -17764,11 +18085,11 @@
       </c>
       <c r="B2" s="11">
         <f>SUMIF(Journal!E2:E978, Résumé!A2,Journal!D2:D978)</f>
-        <v>1.28125</v>
+        <v>1.6701388888888897</v>
       </c>
       <c r="E2" s="18">
         <f>SUM(B2:B7)</f>
-        <v>2.5590277777777777</v>
+        <v>3.0902777777777786</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -17778,7 +18099,7 @@
       </c>
       <c r="B3" s="11">
         <f>SUMIF(Journal!E2:E980, Résumé!A3,Journal!D2:D980)</f>
-        <v>0.42013888888888878</v>
+        <v>0.47569444444444436</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -17798,7 +18119,7 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF(Journal!E2:E982, Résumé!A5,Journal!D2:D982)</f>
-        <v>0.1388888888888889</v>
+        <v>0.15972222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -17808,7 +18129,7 @@
       </c>
       <c r="B6" s="11">
         <f>SUMIF(Journal!E2:E983, Résumé!A6,Journal!D2:D983)</f>
-        <v>0.25347222222222227</v>
+        <v>0.31944444444444442</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>